<commit_message>
add version job finding
</commit_message>
<xml_diff>
--- a/landing-plan.xlsx
+++ b/landing-plan.xlsx
@@ -8,20 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1-Document\document-2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E37F224B-4E36-4FFD-8726-AA0A9CB07C4C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{45857F0A-2DF2-40A3-8924-03FEA049CF0C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="23070" windowHeight="11400" activeTab="2" xr2:uid="{B31260CE-065E-4217-B16B-A0330B6C9870}"/>
+    <workbookView xWindow="6075" yWindow="0" windowWidth="23070" windowHeight="11400" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="plaa" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="离境前计划甘特图" sheetId="3" r:id="rId3"/>
-    <sheet name="物品清单" sheetId="5" r:id="rId4"/>
-    <sheet name="文件清单" sheetId="4" r:id="rId5"/>
-    <sheet name="团聚申请资料清单" sheetId="6" r:id="rId6"/>
-    <sheet name="工作许可资料清单" sheetId="7" r:id="rId7"/>
+    <sheet name="离境前计划甘特图" sheetId="3" r:id="rId1"/>
+    <sheet name="待调查问题" sheetId="8" r:id="rId2"/>
+    <sheet name="物品清单" sheetId="5" r:id="rId3"/>
+    <sheet name="家庭现有物品清单" sheetId="9" r:id="rId4"/>
+    <sheet name="Job-finding" sheetId="11" r:id="rId5"/>
+    <sheet name="生活开支预算" sheetId="10" r:id="rId6"/>
+    <sheet name="文件清单" sheetId="4" r:id="rId7"/>
+    <sheet name="团聚申请资料清单" sheetId="6" r:id="rId8"/>
+    <sheet name="工作许可资料清单" sheetId="7" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">物品清单!$A$1:$H$1</definedName>
+  </definedNames>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +41,7 @@
     <author>yudzhou</author>
   </authors>
   <commentList>
-    <comment ref="C27" authorId="0" shapeId="0" xr:uid="{FA5824C0-CA31-4244-8E72-81D07F5F3E09}">
+    <comment ref="C27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -76,16 +81,182 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Administrator</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Administrator:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+3-生活必需品
+2-生活附加品
+1-非生活必需品</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Administrator:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+3-随身携带
+2-打包携带
+1-个人无法携带</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Administrator:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+4-高于1k
+3-500-1k
+2-200-500
+1-低于200</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>yudzhou</author>
+  </authors>
+  <commentList>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{1C5AC678-D939-46BF-89F0-9DC7CF86423B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>yudzhou:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+username:zhouyuding@icloud.com
+password:Zz12345678~</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{7714C34A-FB92-441A-9303-D237D97C1A2E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>yudzhou:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+username zhouyuding@icloud.com
+Zz12345~</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{2772A692-DAEB-41DB-9F71-57430D397BFB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>yudzhou:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+zhouyuding@icloud.com
+Zz12345~</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
-  <si>
-    <t>aeroplane company</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>route</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="255">
   <si>
     <t>W1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -354,13 +525,565 @@
   <si>
     <t>国内住房交接</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活类</t>
+  </si>
+  <si>
+    <t>萨省的宽带是光纤还是电话线，带什么modem去</t>
+  </si>
+  <si>
+    <t>电器-生活</t>
+  </si>
+  <si>
+    <t>电器-工作</t>
+  </si>
+  <si>
+    <t>衣物</t>
+  </si>
+  <si>
+    <t>药品</t>
+  </si>
+  <si>
+    <t>携带方式</t>
+  </si>
+  <si>
+    <t>使用类型</t>
+  </si>
+  <si>
+    <t>物品</t>
+  </si>
+  <si>
+    <t>详情</t>
+  </si>
+  <si>
+    <t>序列号</t>
+  </si>
+  <si>
+    <t>价值</t>
+  </si>
+  <si>
+    <t>其他</t>
+  </si>
+  <si>
+    <t>牙刷</t>
+  </si>
+  <si>
+    <t>电视</t>
+  </si>
+  <si>
+    <t>音响-huiwei</t>
+  </si>
+  <si>
+    <t>音响-jbl</t>
+  </si>
+  <si>
+    <t>音响-蓝牙接收器</t>
+  </si>
+  <si>
+    <t>吹风机</t>
+  </si>
+  <si>
+    <t>插线板</t>
+  </si>
+  <si>
+    <t>电脑-mac</t>
+  </si>
+  <si>
+    <t>电脑-windows</t>
+  </si>
+  <si>
+    <t>打印机</t>
+  </si>
+  <si>
+    <t>路由器</t>
+  </si>
+  <si>
+    <t>modem</t>
+  </si>
+  <si>
+    <t>待调查，萨省宽带接入方式 光纤 ? 电话线？</t>
+  </si>
+  <si>
+    <t>灯-客厅落地灯</t>
+  </si>
+  <si>
+    <t>灯-床头台灯</t>
+  </si>
+  <si>
+    <t>灯-头戴照明灯</t>
+  </si>
+  <si>
+    <t>灯-小米usb灯</t>
+  </si>
+  <si>
+    <t>充电宝</t>
+  </si>
+  <si>
+    <t>数量</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>家具</t>
+  </si>
+  <si>
+    <t>家电-大家电</t>
+  </si>
+  <si>
+    <t>冰箱</t>
+  </si>
+  <si>
+    <t>洗衣机</t>
+  </si>
+  <si>
+    <t>微波炉</t>
+  </si>
+  <si>
+    <t>烤箱</t>
+  </si>
+  <si>
+    <t>榨汁机</t>
+  </si>
+  <si>
+    <t>电饭煲</t>
+  </si>
+  <si>
+    <t>蒸锅</t>
+  </si>
+  <si>
+    <t>电磁炉</t>
+  </si>
+  <si>
+    <t>区域</t>
+  </si>
+  <si>
+    <t>生活阳台</t>
+  </si>
+  <si>
+    <t>厨房</t>
+  </si>
+  <si>
+    <t>客厅</t>
+  </si>
+  <si>
+    <t>卫生间</t>
+  </si>
+  <si>
+    <t>主卧室</t>
+  </si>
+  <si>
+    <t>次卧室</t>
+  </si>
+  <si>
+    <t>穿鞋凳子</t>
+  </si>
+  <si>
+    <t>鞋子</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>竹架子</t>
+  </si>
+  <si>
+    <t>拖把1</t>
+  </si>
+  <si>
+    <t>小便池</t>
+  </si>
+  <si>
+    <t>衣物篮1</t>
+  </si>
+  <si>
+    <t>电动洗脚盆</t>
+  </si>
+  <si>
+    <t>多用盆（黑）</t>
+  </si>
+  <si>
+    <t>生活阳台置物架</t>
+  </si>
+  <si>
+    <t>小白板</t>
+  </si>
+  <si>
+    <t>空气炸锅</t>
+  </si>
+  <si>
+    <t>飞利浦榨汁机</t>
+  </si>
+  <si>
+    <t>奥克斯破壁机</t>
+  </si>
+  <si>
+    <t>热水壶</t>
+  </si>
+  <si>
+    <t>碗筷架</t>
+  </si>
+  <si>
+    <t>砧板</t>
+  </si>
+  <si>
+    <t>碗筷</t>
+  </si>
+  <si>
+    <t>炒锅</t>
+  </si>
+  <si>
+    <t>煮锅</t>
+  </si>
+  <si>
+    <t>平底锅</t>
+  </si>
+  <si>
+    <t>超薄平底锅</t>
+  </si>
+  <si>
+    <t>烤肉炉</t>
+  </si>
+  <si>
+    <t>多用途烤肉板</t>
+  </si>
+  <si>
+    <t>电子秤</t>
+  </si>
+  <si>
+    <t>ikea玻璃容器</t>
+  </si>
+  <si>
+    <t>ikea厨房抽屉容器</t>
+  </si>
+  <si>
+    <t>ikea塑料瓶装塑料容器</t>
+  </si>
+  <si>
+    <t>净水器</t>
+  </si>
+  <si>
+    <t>可挪动铁支架</t>
+  </si>
+  <si>
+    <t>餐厅</t>
+  </si>
+  <si>
+    <t>饭桌</t>
+  </si>
+  <si>
+    <t>木质椅子</t>
+  </si>
+  <si>
+    <t>红色铁支架</t>
+  </si>
+  <si>
+    <t>藤编容器篮</t>
+  </si>
+  <si>
+    <t>4+2</t>
+  </si>
+  <si>
+    <t>纸箱杂物-餐厅</t>
+  </si>
+  <si>
+    <t>斗柜</t>
+  </si>
+  <si>
+    <t>斗柜内杂物</t>
+  </si>
+  <si>
+    <t>电视机</t>
+  </si>
+  <si>
+    <t>多人沙发</t>
+  </si>
+  <si>
+    <t>单人沙发</t>
+  </si>
+  <si>
+    <t>电脑桌</t>
+  </si>
+  <si>
+    <t>惠威音响</t>
+  </si>
+  <si>
+    <t>DDJ-SB2</t>
+  </si>
+  <si>
+    <t>蓝牙接收器</t>
+  </si>
+  <si>
+    <t>照片</t>
+  </si>
+  <si>
+    <t xml:space="preserve">冰箱贴 </t>
+  </si>
+  <si>
+    <t>刀具/厨房小工具</t>
+  </si>
+  <si>
+    <t>黑色茶几</t>
+  </si>
+  <si>
+    <t>阳台</t>
+  </si>
+  <si>
+    <t>书桌</t>
+  </si>
+  <si>
+    <t>显示器</t>
+  </si>
+  <si>
+    <t>书籍</t>
+  </si>
+  <si>
+    <t>电竞椅</t>
+  </si>
+  <si>
+    <t>电脑配件(鼠标、键盘)</t>
+  </si>
+  <si>
+    <t>电子设备小型配件（usb线、读卡器、内存卡 等位于书桌上）</t>
+  </si>
+  <si>
+    <t>玩偶</t>
+  </si>
+  <si>
+    <t>立柜下柜杂物</t>
+  </si>
+  <si>
+    <t>立柜杂物-药品</t>
+  </si>
+  <si>
+    <t>立柜杂物-文件</t>
+  </si>
+  <si>
+    <t>立柜杂物-其他</t>
+  </si>
+  <si>
+    <t>圣诞树</t>
+  </si>
+  <si>
+    <t>DJ Controller支架</t>
+  </si>
+  <si>
+    <t>拖把2</t>
+  </si>
+  <si>
+    <t>塑料白色可挪动置物架</t>
+  </si>
+  <si>
+    <t>红色小凳</t>
+  </si>
+  <si>
+    <t>软包凳</t>
+  </si>
+  <si>
+    <t>淋浴房置物架杂物</t>
+  </si>
+  <si>
+    <t>隔板置物架杂物</t>
+  </si>
+  <si>
+    <t>台盆上杂物</t>
+  </si>
+  <si>
+    <t>夹板</t>
+  </si>
+  <si>
+    <t>台盆下杂物</t>
+  </si>
+  <si>
+    <t>洗漱柜内杂物</t>
+  </si>
+  <si>
+    <t>电暖气</t>
+  </si>
+  <si>
+    <t>水暖气</t>
+  </si>
+  <si>
+    <t>床</t>
+  </si>
+  <si>
+    <t>床头灯</t>
+  </si>
+  <si>
+    <t>衣服立挂支架</t>
+  </si>
+  <si>
+    <t>白色衣物架</t>
+  </si>
+  <si>
+    <t>白色衣物架下-杂物</t>
+  </si>
+  <si>
+    <t>床头柜杂物</t>
+  </si>
+  <si>
+    <t>温度计</t>
+  </si>
+  <si>
+    <t>落地灯</t>
+  </si>
+  <si>
+    <t>电力猫</t>
+  </si>
+  <si>
+    <t>插板</t>
+  </si>
+  <si>
+    <t>朱红色小书桌</t>
+  </si>
+  <si>
+    <t>黑色迷你书桌</t>
+  </si>
+  <si>
+    <t>油汀</t>
+  </si>
+  <si>
+    <t>电风扇</t>
+  </si>
+  <si>
+    <t>红色迷你书桌</t>
+  </si>
+  <si>
+    <t>钢架床</t>
+  </si>
+  <si>
+    <t>电热毯</t>
+  </si>
+  <si>
+    <t>床下柜杂物-背包</t>
+  </si>
+  <si>
+    <t>床下柜杂物-救生绳子</t>
+  </si>
+  <si>
+    <t>床下柜杂物-压缩袋</t>
+  </si>
+  <si>
+    <t>床下柜杂物-其他</t>
+  </si>
+  <si>
+    <t>地毯</t>
+  </si>
+  <si>
+    <t>懒人沙发</t>
+  </si>
+  <si>
+    <t>被褥/床单/枕头 等床上用品-主卧室</t>
+  </si>
+  <si>
+    <t>被褥/床单/枕头 等床上用品-次卧室</t>
+  </si>
+  <si>
+    <t>衣柜-衣物-次卧室</t>
+  </si>
+  <si>
+    <t>衣柜-杂物-次卧室</t>
+  </si>
+  <si>
+    <t>衣柜-杂物-主卧室</t>
+  </si>
+  <si>
+    <t>衣柜-衣物-主卧室</t>
+  </si>
+  <si>
+    <t>奖章/纪念品等杂物</t>
+  </si>
+  <si>
+    <t>生活必需品优先级</t>
+  </si>
+  <si>
+    <t>携带难易指数</t>
+  </si>
+  <si>
+    <t>价值高低优先级</t>
+  </si>
+  <si>
+    <t>taking factor</t>
+  </si>
+  <si>
+    <t>饮食</t>
+  </si>
+  <si>
+    <t>住宿</t>
+  </si>
+  <si>
+    <t>交通</t>
+  </si>
+  <si>
+    <t>site</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>company</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>job description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.northstarats.com/SED-Systems/Intermediate-Software-Developer-Sirius-XM/45464/1346870</t>
+  </si>
+  <si>
+    <t>https://www.northstarats.com/SED-Systems/Senior-Software-Developer-Sirius-XM/45462/1346869</t>
+  </si>
+  <si>
+    <t>application detail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.northstarats.com/SED-Systems/MyApplications</t>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>03/06/2019</t>
+  </si>
+  <si>
+    <t>https://www.northstarats.com/SED-Systems/Entry-Level-Software-Developer-New-Grad-Opportunity/45609/1346872</t>
+  </si>
+  <si>
+    <t>https://chc.tbe.taleo.net/chc01/ats/careers/v2/myJobs?org=MENTOR&amp;cws=44</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.ca/partner/jobListing.htm?pos=102&amp;ao=201328&amp;s=58&amp;guid=0000016952d86086a817e0bd1d714842&amp;src=GD_JOB_AD&amp;t=SR&amp;extid=1&amp;exst=OL&amp;ist=&amp;ast=OL&amp;vt=w&amp;slr=true&amp;cs=1_bd70350f&amp;cb=1551873106593&amp;jobListingId=2950423839</t>
+  </si>
+  <si>
+    <t>https://ca.indeed.com/viewjob?jk=1037f8afd6867b35&amp;tk=1d59gmbb10k5a003&amp;from=serp&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://ca.indeed.com/viewjob?jk=8d993087c33dff04&amp;tk=1d59gmbb10k5a003&amp;from=serp&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://www.indeed.ca/cmp/Yardi-Canada-Ltd.-(Point2)/jobs/Software-Developer-553a80bc375edd7b?q=software&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://ca.indeed.com/viewjob?jk=35fd915ddafa0eb1&amp;tk=1d59is47a0k5a002&amp;from=serp&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>https://csc.wd1.myworkdayjobs.com/en-US/DXCJobs/jobs</t>
+  </si>
+  <si>
+    <t>https://ca.indeed.com/viewjob?jk=d2c665ae071a6ea7&amp;tk=1d59is47a0k5a002&amp;from=serp&amp;vjs=3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,6 +1126,20 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF393838"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -448,7 +1185,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -458,7 +1195,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
@@ -470,7 +1207,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -479,10 +1216,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -500,116 +1243,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Climate graph // Weather by Month, Saskatoon">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E815E715-CA6F-42F1-91F0-3AA4FA509C92}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2400300" y="581025"/>
-          <a:ext cx="7762875" cy="5819775"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>189530</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>104048</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3E111BC-2FA7-46E6-80D7-2EEC1FFFAAF8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5457825" y="619125"/>
-          <a:ext cx="7761905" cy="5819048"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -908,59 +1541,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1A6F728-D995-48A5-A47E-83EA6D30D2B8}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F082416D-8815-4ED2-AA6E-239F6CF4F833}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5027C885-7D4B-449D-999F-8681634DD17F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ED31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V17" sqref="V17"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -971,9 +1559,7 @@
     <col min="6" max="7" width="2.625" style="8" customWidth="1"/>
     <col min="8" max="9" width="2.625" customWidth="1"/>
     <col min="10" max="10" width="2.625" style="8" customWidth="1"/>
-    <col min="11" max="13" width="2.625" customWidth="1"/>
-    <col min="14" max="14" width="2.625" style="8" customWidth="1"/>
-    <col min="15" max="28" width="2.625" customWidth="1"/>
+    <col min="11" max="28" width="2.625" customWidth="1"/>
     <col min="29" max="29" width="2.625" style="8" customWidth="1"/>
     <col min="30" max="75" width="2.625" customWidth="1"/>
     <col min="76" max="76" width="2.625" style="6" customWidth="1"/>
@@ -982,108 +1568,108 @@
   <sheetData>
     <row r="1" spans="1:134" x14ac:dyDescent="0.2">
       <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="N1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="R1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="V1" t="s">
         <v>22</v>
       </c>
-      <c r="R1" t="s">
+      <c r="Z1" t="s">
         <v>23</v>
-      </c>
-      <c r="V1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:134" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="L2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="P2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="W2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AC2" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:134" s="2" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1117,7 +1703,7 @@
       <c r="M3" s="3">
         <v>43525</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="3">
         <v>43526</v>
       </c>
       <c r="O3" s="3">
@@ -1483,7 +2069,7 @@
     </row>
     <row r="4" spans="1:134" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="9"/>
@@ -1494,7 +2080,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="9"/>
+      <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -1528,7 +2114,7 @@
     </row>
     <row r="5" spans="1:134" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AD5" s="4"/>
       <c r="AE5" s="4"/>
@@ -1548,13 +2134,13 @@
     </row>
     <row r="6" spans="1:134" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>67</v>
-      </c>
-      <c r="N6" s="11"/>
+        <v>65</v>
+      </c>
+      <c r="AC6" s="11"/>
     </row>
     <row r="7" spans="1:134" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
@@ -1574,7 +2160,7 @@
     </row>
     <row r="9" spans="1:134" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AD9" s="4"/>
       <c r="AE9" s="4"/>
@@ -1594,7 +2180,7 @@
     </row>
     <row r="11" spans="1:134" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AD11" s="4"/>
       <c r="AE11" s="4"/>
@@ -1614,7 +2200,7 @@
     </row>
     <row r="13" spans="1:134" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AD13" s="4"/>
       <c r="AE13" s="4"/>
@@ -1634,7 +2220,7 @@
     </row>
     <row r="14" spans="1:134" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AS14" s="4"/>
       <c r="AT14" s="4"/>
@@ -1653,7 +2239,7 @@
     </row>
     <row r="15" spans="1:134" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AD15" s="4"/>
       <c r="AE15" s="4"/>
@@ -1673,7 +2259,7 @@
     </row>
     <row r="17" spans="3:75" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1685,7 +2271,7 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
-      <c r="N17" s="11"/>
+      <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
@@ -1695,7 +2281,7 @@
     </row>
     <row r="18" spans="3:75" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AS18" s="5"/>
       <c r="AT18" s="5"/>
@@ -1717,7 +2303,7 @@
     </row>
     <row r="19" spans="3:75" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -1729,7 +2315,7 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
-      <c r="N19" s="11"/>
+      <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
@@ -1739,7 +2325,7 @@
     </row>
     <row r="20" spans="3:75" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
@@ -1784,12 +2370,12 @@
     </row>
     <row r="22" spans="3:75" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="3:75" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AD24" s="4"/>
       <c r="AE24" s="4"/>
@@ -1809,7 +2395,7 @@
     </row>
     <row r="25" spans="3:75" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1821,7 +2407,7 @@
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
-      <c r="N25" s="11"/>
+      <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
@@ -1831,12 +2417,12 @@
     </row>
     <row r="26" spans="3:75" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="3:75" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -1848,7 +2434,7 @@
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
-      <c r="N27" s="11"/>
+      <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
@@ -1866,7 +2452,7 @@
     </row>
     <row r="28" spans="3:75" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="AD28" s="4"/>
       <c r="AE28" s="4"/>
@@ -1879,12 +2465,12 @@
     </row>
     <row r="29" spans="3:75" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="3:75" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AD30" s="4"/>
       <c r="AE30" s="4"/>
@@ -1918,7 +2504,7 @@
     </row>
     <row r="31" spans="3:75" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="BG31" s="4"/>
       <c r="BH31" s="4"/>
@@ -1946,24 +2532,1520 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D620FDB-DB89-4B40-A1E8-A2B4F20510E3}">
-  <dimension ref="A1:A3"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:L133"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.75" customWidth="1"/>
+    <col min="3" max="3" width="22.75" customWidth="1"/>
+    <col min="5" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J1" t="s">
+        <v>230</v>
+      </c>
+      <c r="K1" t="s">
+        <v>231</v>
+      </c>
+      <c r="L1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" t="s">
+        <v>139</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" t="s">
+        <v>143</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" t="s">
+        <v>145</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" t="s">
+        <v>146</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" t="s">
+        <v>171</v>
+      </c>
+      <c r="D36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" t="s">
+        <v>150</v>
+      </c>
+      <c r="D38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" t="s">
+        <v>148</v>
+      </c>
+      <c r="D39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" t="s">
+        <v>149</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" t="s">
+        <v>170</v>
+      </c>
+      <c r="D43" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>153</v>
+      </c>
+      <c r="C45" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>153</v>
+      </c>
+      <c r="C46" t="s">
+        <v>155</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>153</v>
+      </c>
+      <c r="C47" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>153</v>
+      </c>
+      <c r="C49" t="s">
+        <v>157</v>
+      </c>
+      <c r="D49" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>153</v>
+      </c>
+      <c r="C50" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>153</v>
+      </c>
+      <c r="C51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D51" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>119</v>
+      </c>
+      <c r="C52" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>119</v>
+      </c>
+      <c r="C53" t="s">
+        <v>169</v>
+      </c>
+      <c r="D53" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>119</v>
+      </c>
+      <c r="C54" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C56" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>119</v>
+      </c>
+      <c r="C57" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>119</v>
+      </c>
+      <c r="C63" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>119</v>
+      </c>
+      <c r="C64" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>119</v>
+      </c>
+      <c r="C65" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>119</v>
+      </c>
+      <c r="C66" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>119</v>
+      </c>
+      <c r="C67" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>119</v>
+      </c>
+      <c r="C69" t="s">
+        <v>208</v>
+      </c>
+      <c r="D69" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>173</v>
+      </c>
+      <c r="C71" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>173</v>
+      </c>
+      <c r="C72" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>173</v>
+      </c>
+      <c r="C73" t="s">
+        <v>176</v>
+      </c>
+      <c r="D73" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>173</v>
+      </c>
+      <c r="C74" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>173</v>
+      </c>
+      <c r="C75" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>173</v>
+      </c>
+      <c r="C76" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>173</v>
+      </c>
+      <c r="C77" t="s">
+        <v>228</v>
+      </c>
+      <c r="D77" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>173</v>
+      </c>
+      <c r="C78" t="s">
+        <v>180</v>
+      </c>
+      <c r="D78" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>173</v>
+      </c>
+      <c r="C79" t="s">
+        <v>181</v>
+      </c>
+      <c r="D79" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>173</v>
+      </c>
+      <c r="C80" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>173</v>
+      </c>
+      <c r="C81" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>173</v>
+      </c>
+      <c r="C82" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>173</v>
+      </c>
+      <c r="C83" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>173</v>
+      </c>
+      <c r="C84" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>173</v>
+      </c>
+      <c r="C85" t="s">
+        <v>190</v>
+      </c>
+      <c r="D85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>120</v>
+      </c>
+      <c r="C91" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>120</v>
+      </c>
+      <c r="C92" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>120</v>
+      </c>
+      <c r="C93" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>120</v>
+      </c>
+      <c r="C94" t="s">
+        <v>191</v>
+      </c>
+      <c r="D94" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>120</v>
+      </c>
+      <c r="C95" t="s">
+        <v>192</v>
+      </c>
+      <c r="D95" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>120</v>
+      </c>
+      <c r="C96" t="s">
+        <v>193</v>
+      </c>
+      <c r="D96" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>120</v>
+      </c>
+      <c r="C97" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>120</v>
+      </c>
+      <c r="C98" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>120</v>
+      </c>
+      <c r="C99" t="s">
+        <v>195</v>
+      </c>
+      <c r="D99" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>120</v>
+      </c>
+      <c r="C100" t="s">
+        <v>196</v>
+      </c>
+      <c r="D100" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>121</v>
+      </c>
+      <c r="C107" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>121</v>
+      </c>
+      <c r="C108" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>121</v>
+      </c>
+      <c r="C109" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>121</v>
+      </c>
+      <c r="C110" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>121</v>
+      </c>
+      <c r="C111" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>121</v>
+      </c>
+      <c r="C112" t="s">
+        <v>204</v>
+      </c>
+      <c r="D112" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>121</v>
+      </c>
+      <c r="C113" t="s">
+        <v>227</v>
+      </c>
+      <c r="D113" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>121</v>
+      </c>
+      <c r="C114" t="s">
+        <v>226</v>
+      </c>
+      <c r="D114" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>121</v>
+      </c>
+      <c r="C115" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>121</v>
+      </c>
+      <c r="C116" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>121</v>
+      </c>
+      <c r="C117" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>121</v>
+      </c>
+      <c r="C118" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>121</v>
+      </c>
+      <c r="C119" t="s">
+        <v>222</v>
+      </c>
+      <c r="D119" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>121</v>
+      </c>
+      <c r="C120" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>121</v>
+      </c>
+      <c r="C121" t="s">
+        <v>216</v>
+      </c>
+      <c r="D121">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>121</v>
+      </c>
+      <c r="C122" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>121</v>
+      </c>
+      <c r="C123" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>121</v>
+      </c>
+      <c r="C124" t="s">
+        <v>219</v>
+      </c>
+      <c r="D124" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>122</v>
+      </c>
+      <c r="C125" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>122</v>
+      </c>
+      <c r="C126" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>122</v>
+      </c>
+      <c r="C127" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>122</v>
+      </c>
+      <c r="C128" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>122</v>
+      </c>
+      <c r="C129" t="s">
+        <v>220</v>
+      </c>
+      <c r="D129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>122</v>
+      </c>
+      <c r="C130" t="s">
+        <v>221</v>
+      </c>
+      <c r="D130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>122</v>
+      </c>
+      <c r="C131" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>122</v>
+      </c>
+      <c r="C132" t="s">
+        <v>224</v>
+      </c>
+      <c r="D132" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>122</v>
+      </c>
+      <c r="C133" t="s">
+        <v>225</v>
+      </c>
+      <c r="D133" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D209D96D-824B-457C-A571-11231482512B}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="98.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D3" t="s">
+        <v>243</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" t="s">
+        <v>243</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>252</v>
+      </c>
+      <c r="D9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C10" s="13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="B1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>41</v>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>1200</v>
       </c>
     </row>
   </sheetData>
@@ -1973,8 +4055,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1AA1480-4A69-47B9-BD54-3BDA8C04137D}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1989,67 +4071,67 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
         <v>52</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2059,8 +4141,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367617DA-4BB8-4BDB-9223-0BDD0047141F}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2073,8 +4155,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE458399-3C80-46AE-97F1-9DEBF47F4AC4}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>